<commit_message>
[Freight_Journal] : Test Data Add
</commit_message>
<xml_diff>
--- a/Test_data/Freight_Journal.xlsx
+++ b/Test_data/Freight_Journal.xlsx
@@ -263,7 +263,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="271">
   <si>
     <t>ID</t>
   </si>
@@ -1057,34 +1057,25 @@
     <t>KTS00057</t>
   </si>
   <si>
-    <t>MUM/BKG/AEC/00012/2122-60</t>
+    <t>10-Jul-2023</t>
+  </si>
+  <si>
+    <t>01-Jul-2023</t>
+  </si>
+  <si>
+    <t>30-Jul-2023</t>
+  </si>
+  <si>
+    <t>06-Jul-2023</t>
+  </si>
+  <si>
+    <t>KTS00062</t>
+  </si>
+  <si>
+    <t>KTS00063</t>
   </si>
   <si>
     <t>CHN/BKG/AFI/00191/23-24</t>
-  </si>
-  <si>
-    <t>03-Jul-2023</t>
-  </si>
-  <si>
-    <t>CHN/BKG/AFE/00190/23-24</t>
-  </si>
-  <si>
-    <t>05-Jul-2023</t>
-  </si>
-  <si>
-    <t>10-Jul-2023</t>
-  </si>
-  <si>
-    <t>KTS00060</t>
-  </si>
-  <si>
-    <t>KTS00061</t>
-  </si>
-  <si>
-    <t>01-Jul-2023</t>
-  </si>
-  <si>
-    <t>30-Jul-2023</t>
   </si>
 </sst>
 </file>
@@ -2048,7 +2039,7 @@
   <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2200,7 +2191,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="36">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C8" s="37" t="s">
         <v>17</v>
@@ -2256,7 +2247,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="46">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C10" s="47" t="s">
         <v>17</v>
@@ -2385,7 +2376,7 @@
   <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView zoomScale="108" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2522,7 +2513,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="39">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C8" s="37" t="s">
         <v>239</v>
@@ -2540,16 +2531,16 @@
         <v>29</v>
       </c>
       <c r="H8" s="62" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="I8" s="62" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="J8" s="62" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="K8" s="37" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="L8" s="38" t="s">
         <v>229</v>
@@ -2578,16 +2569,16 @@
         <v>29</v>
       </c>
       <c r="H9" s="63" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="I9" s="63" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="J9" s="63" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="K9" s="42" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L9" s="44" t="s">
         <v>260</v>
@@ -2596,7 +2587,7 @@
     <row r="10" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="46">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C10" s="47" t="s">
         <v>240</v>
@@ -2764,7 +2755,7 @@
   <dimension ref="A1:GF13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3441,16 +3432,14 @@
         <v>9</v>
       </c>
       <c r="B8" s="65">
-        <v>1</v>
-      </c>
-      <c r="C8" s="73" t="s">
-        <v>267</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C8" s="73"/>
       <c r="D8" s="69" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="E8" s="62" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="F8" s="52" t="s">
         <v>235</v>
@@ -3486,11 +3475,9 @@
       <c r="B9" s="66">
         <v>2</v>
       </c>
-      <c r="C9" s="60" t="s">
-        <v>264</v>
-      </c>
+      <c r="C9" s="60"/>
       <c r="D9" s="70" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="E9" s="63" t="s">
         <v>246</v>
@@ -3527,16 +3514,16 @@
         <v>11</v>
       </c>
       <c r="B10" s="67">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C10" s="72" t="s">
+        <v>270</v>
+      </c>
+      <c r="D10" s="71" t="s">
         <v>265</v>
       </c>
-      <c r="D10" s="71" t="s">
-        <v>272</v>
-      </c>
       <c r="E10" s="64" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="F10" s="32" t="s">
         <v>217</v>

</xml_diff>

<commit_message>
[Freight_Journal] : Change in Test Data
</commit_message>
<xml_diff>
--- a/Test_data/Freight_Journal.xlsx
+++ b/Test_data/Freight_Journal.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="NewFreightJournal" sheetId="1" r:id="rId1"/>
@@ -263,7 +263,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="272">
   <si>
     <t>ID</t>
   </si>
@@ -1057,25 +1057,28 @@
     <t>KTS00057</t>
   </si>
   <si>
-    <t>10-Jul-2023</t>
-  </si>
-  <si>
     <t>01-Jul-2023</t>
   </si>
   <si>
     <t>30-Jul-2023</t>
   </si>
   <si>
-    <t>06-Jul-2023</t>
-  </si>
-  <si>
-    <t>KTS00062</t>
-  </si>
-  <si>
-    <t>KTS00063</t>
-  </si>
-  <si>
-    <t>CHN/BKG/AFI/00191/23-24</t>
+    <t>14-Jul-2023</t>
+  </si>
+  <si>
+    <t>20-Jul-2023</t>
+  </si>
+  <si>
+    <t>KTS00064</t>
+  </si>
+  <si>
+    <t>KTS00065</t>
+  </si>
+  <si>
+    <t>CHN/BKG/AFE/00196/23-24</t>
+  </si>
+  <si>
+    <t>MUM/BKG/AEC/00012/2122-62</t>
   </si>
 </sst>
 </file>
@@ -2039,7 +2042,7 @@
   <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2191,7 +2194,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="36">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C8" s="37" t="s">
         <v>17</v>
@@ -2247,7 +2250,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="46">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C10" s="47" t="s">
         <v>17</v>
@@ -2375,8 +2378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView zoomScale="108" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2513,7 +2516,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="39">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C8" s="37" t="s">
         <v>239</v>
@@ -2531,13 +2534,13 @@
         <v>29</v>
       </c>
       <c r="H8" s="62" t="s">
+        <v>266</v>
+      </c>
+      <c r="I8" s="62" t="s">
         <v>267</v>
       </c>
-      <c r="I8" s="62" t="s">
-        <v>264</v>
-      </c>
       <c r="J8" s="62" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K8" s="37" t="s">
         <v>268</v>
@@ -2569,13 +2572,13 @@
         <v>29</v>
       </c>
       <c r="H9" s="63" t="s">
+        <v>266</v>
+      </c>
+      <c r="I9" s="63" t="s">
         <v>267</v>
       </c>
-      <c r="I9" s="63" t="s">
-        <v>264</v>
-      </c>
       <c r="J9" s="63" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K9" s="42" t="s">
         <v>269</v>
@@ -2587,7 +2590,7 @@
     <row r="10" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="46">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C10" s="47" t="s">
         <v>240</v>
@@ -2754,8 +2757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GF13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3432,14 +3435,16 @@
         <v>9</v>
       </c>
       <c r="B8" s="65">
-        <v>3</v>
-      </c>
-      <c r="C8" s="73"/>
+        <v>1</v>
+      </c>
+      <c r="C8" s="73" t="s">
+        <v>270</v>
+      </c>
       <c r="D8" s="69" t="s">
+        <v>264</v>
+      </c>
+      <c r="E8" s="62" t="s">
         <v>265</v>
-      </c>
-      <c r="E8" s="62" t="s">
-        <v>266</v>
       </c>
       <c r="F8" s="52" t="s">
         <v>235</v>
@@ -3475,9 +3480,11 @@
       <c r="B9" s="66">
         <v>2</v>
       </c>
-      <c r="C9" s="60"/>
+      <c r="C9" s="60" t="s">
+        <v>271</v>
+      </c>
       <c r="D9" s="70" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E9" s="63" t="s">
         <v>246</v>
@@ -3514,16 +3521,14 @@
         <v>11</v>
       </c>
       <c r="B10" s="67">
-        <v>1</v>
-      </c>
-      <c r="C10" s="72" t="s">
-        <v>270</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C10" s="72"/>
       <c r="D10" s="71" t="s">
+        <v>264</v>
+      </c>
+      <c r="E10" s="64" t="s">
         <v>265</v>
-      </c>
-      <c r="E10" s="64" t="s">
-        <v>266</v>
       </c>
       <c r="F10" s="32" t="s">
         <v>217</v>

</xml_diff>